<commit_message>
refactor(comment): update comment creation tests to use findById and improve verification update tasklog
</commit_message>
<xml_diff>
--- a/documentation/IAA-Tasklog-Gruppe11-LarsNicht.xlsx
+++ b/documentation/IAA-Tasklog-Gruppe11-LarsNicht.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Tasklog</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Aktualisierung README / Projektübersicht und Installationsanleitung.</t>
+  </si>
+  <si>
+    <t>Fix tests for bugfix</t>
   </si>
   <si>
     <t>Summe</t>
@@ -1222,9 +1225,15 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" ht="25.5" customHeight="1">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
+      <c r="A22" s="10">
+        <v>45975.0</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="13">
+        <v>1.0</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -2008,11 +2017,11 @@
     <row r="50" ht="25.5" customHeight="1">
       <c r="A50" s="19"/>
       <c r="B50" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C50" s="21">
         <f>SUM(C3:C49)</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>

</xml_diff>

<commit_message>
feat(project): enforce unique and uppercase abbreviation for projects add exception handling for open tickets when deleting a project make projects only deletable when all tickets are closed
</commit_message>
<xml_diff>
--- a/documentation/IAA-Tasklog-Gruppe11-LarsNicht.xlsx
+++ b/documentation/IAA-Tasklog-Gruppe11-LarsNicht.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Tasklog</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Fix tests for bugfix</t>
+  </si>
+  <si>
+    <t>Projektkürzel unique und in Capital, projekt erst löschen wenn alle tickets geschlossen, tests</t>
   </si>
   <si>
     <t>Summe</t>
@@ -1259,9 +1262,15 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" ht="25.5" customHeight="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
+      <c r="A23" s="10">
+        <v>45976.0</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1.5</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1289,7 +1298,7 @@
     <row r="24" ht="25.5" customHeight="1">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="16"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1317,7 +1326,7 @@
     <row r="25" ht="25.5" customHeight="1">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1345,7 +1354,7 @@
     <row r="26" ht="25.5" customHeight="1">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1373,7 +1382,7 @@
     <row r="27" ht="25.5" customHeight="1">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1401,7 +1410,7 @@
     <row r="28" ht="25.5" customHeight="1">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="16"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1429,7 +1438,7 @@
     <row r="29" ht="25.5" customHeight="1">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
-      <c r="C29" s="16"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1457,7 +1466,7 @@
     <row r="30" ht="25.5" customHeight="1">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1485,7 +1494,7 @@
     <row r="31" ht="25.5" customHeight="1">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1513,7 +1522,7 @@
     <row r="32" ht="25.5" customHeight="1">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1541,7 +1550,7 @@
     <row r="33" ht="25.5" customHeight="1">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
-      <c r="C33" s="16"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1569,7 +1578,7 @@
     <row r="34" ht="25.5" customHeight="1">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1597,7 +1606,7 @@
     <row r="35" ht="25.5" customHeight="1">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1625,7 +1634,7 @@
     <row r="36" ht="25.5" customHeight="1">
       <c r="A36" s="16"/>
       <c r="B36" s="15"/>
-      <c r="C36" s="16"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1653,7 +1662,7 @@
     <row r="37" ht="25.5" customHeight="1">
       <c r="A37" s="16"/>
       <c r="B37" s="15"/>
-      <c r="C37" s="16"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1681,7 +1690,7 @@
     <row r="38" ht="25.5" customHeight="1">
       <c r="A38" s="16"/>
       <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1709,7 +1718,7 @@
     <row r="39" ht="25.5" customHeight="1">
       <c r="A39" s="16"/>
       <c r="B39" s="15"/>
-      <c r="C39" s="16"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1737,7 +1746,7 @@
     <row r="40" ht="25.5" customHeight="1">
       <c r="A40" s="16"/>
       <c r="B40" s="15"/>
-      <c r="C40" s="16"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1765,7 +1774,7 @@
     <row r="41" ht="25.5" customHeight="1">
       <c r="A41" s="16"/>
       <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1793,7 +1802,7 @@
     <row r="42" ht="25.5" customHeight="1">
       <c r="A42" s="16"/>
       <c r="B42" s="15"/>
-      <c r="C42" s="16"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1821,7 +1830,7 @@
     <row r="43" ht="25.5" customHeight="1">
       <c r="A43" s="16"/>
       <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1849,7 +1858,7 @@
     <row r="44" ht="25.5" customHeight="1">
       <c r="A44" s="16"/>
       <c r="B44" s="15"/>
-      <c r="C44" s="16"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1877,7 +1886,7 @@
     <row r="45" ht="25.5" customHeight="1">
       <c r="A45" s="16"/>
       <c r="B45" s="15"/>
-      <c r="C45" s="16"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -1905,7 +1914,7 @@
     <row r="46" ht="25.5" customHeight="1">
       <c r="A46" s="16"/>
       <c r="B46" s="15"/>
-      <c r="C46" s="16"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -2017,11 +2026,11 @@
     <row r="50" ht="25.5" customHeight="1">
       <c r="A50" s="19"/>
       <c r="B50" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C50" s="21">
         <f>SUM(C3:C49)</f>
-        <v>69</v>
+        <v>70.5</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>

</xml_diff>